<commit_message>
add new data for testing in excel format to the repo
</commit_message>
<xml_diff>
--- a/data/input/pilot.xlsx
+++ b/data/input/pilot.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="15255" windowHeight="5385" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="15255" windowHeight="5385" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="จัดฟัน" sheetId="1" r:id="rId1"/>
     <sheet name="ไม่จัดฟัน" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="ใช้ทดสอบ" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="19">
   <si>
     <t>DN</t>
   </si>
@@ -64,6 +64,15 @@
   </si>
   <si>
     <t>missing</t>
+  </si>
+  <si>
+    <t>หมายเหตุ</t>
+  </si>
+  <si>
+    <t>จัดฟัน</t>
+  </si>
+  <si>
+    <t>ไม่จัดฟัน</t>
   </si>
 </sst>
 </file>
@@ -398,8 +407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1248,7 +1257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
@@ -1930,12 +1939,206 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
+  <cols>
+    <col min="14" max="14" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2">
+        <v>2.5</v>
+      </c>
+      <c r="K2">
+        <v>3.5</v>
+      </c>
+      <c r="L2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2">
+        <v>2</v>
+      </c>
+      <c r="O2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3">
+        <v>3.5</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="L3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1.5</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>